<commit_message>
adding macro command to read cdte ring buffer
</commit_message>
<xml_diff>
--- a/cdte1_command_deck.xlsx
+++ b/cdte1_command_deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thanasi/Documents/FOXSI/Data/formatter/foxsi4-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0072FCF8-425A-0A4E-BF88-FCC024775E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A55E31E5-1BCB-E943-A77C-85DD67A3C2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17920" xr2:uid="{1DE950B2-129E-5A4D-8896-FB78BBCF4CAC}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="144">
   <si>
     <t>R=1/W=0</t>
   </si>
@@ -276,39 +276,9 @@
     <t>0x3c3c0100040404043c3c3c3c</t>
   </si>
   <si>
-    <t>read_de_pi_temp</t>
-  </si>
-  <si>
-    <t>0x00000010</t>
-  </si>
-  <si>
-    <t>read_can_ping_status</t>
-  </si>
-  <si>
-    <t>0x0000000c</t>
-  </si>
-  <si>
-    <t>read temperature of Raspberry Pi CPU in ºC</t>
-  </si>
-  <si>
-    <t>read_de_cpu_usage</t>
-  </si>
-  <si>
-    <t>usage</t>
-  </si>
-  <si>
-    <t>0x00000014</t>
-  </si>
-  <si>
     <t>read DE status control register</t>
   </si>
   <si>
-    <t>read DE Raspberry Pi CPU usage (percentage)</t>
-  </si>
-  <si>
-    <t>read ping status of each canister</t>
-  </si>
-  <si>
     <t>set_can1_idle</t>
   </si>
   <si>
@@ -490,6 +460,12 @@
   </si>
   <si>
     <t>canister 1 will show status in DE terminal (for debug)</t>
+  </si>
+  <si>
+    <t>read_can1_events</t>
+  </si>
+  <si>
+    <t>read MACRO for event data in ring buffer from canister (see Formatter implementation)</t>
   </si>
 </sst>
 </file>
@@ -961,13 +937,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{283F008E-2DBD-E446-BC2F-AA0D9FF4122A}">
-  <dimension ref="A1:AC40"/>
+  <dimension ref="A1:AC38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomRight" activeCell="AD18" sqref="AD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1111,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="3" t="str">
-        <f t="shared" ref="E3:E21" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
+        <f t="shared" ref="E3:E19" si="0">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C3,7) + BIN2DEC($D3)))</f>
         <v>0x80</v>
       </c>
       <c r="F3" s="3" t="s">
@@ -1393,7 +1369,7 @@
     </row>
     <row r="6" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>55</v>
@@ -1405,7 +1381,7 @@
         <v>100000</v>
       </c>
       <c r="E6" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C6,7) + BIN2DEC($D6)))</f>
+        <f t="shared" ref="E6:E17" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C6,7) + BIN2DEC($D6)))</f>
         <v>0xA0</v>
       </c>
       <c r="F6" s="3" t="s">
@@ -1469,7 +1445,7 @@
         <v>73</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="AA6" s="25" t="s">
         <v>41</v>
@@ -1478,12 +1454,12 @@
         <v>69</v>
       </c>
       <c r="AC6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>55</v>
@@ -1495,7 +1471,7 @@
         <v>100010</v>
       </c>
       <c r="E7" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C7,7) + BIN2DEC($D7)))</f>
+        <f t="shared" si="1"/>
         <v>0xA2</v>
       </c>
       <c r="F7" s="3" t="s">
@@ -1511,7 +1487,7 @@
         <v>17</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="K7" s="23" t="s">
         <v>70</v>
@@ -1559,7 +1535,7 @@
         <v>73</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="AA7" s="25" t="s">
         <v>41</v>
@@ -1568,12 +1544,12 @@
         <v>69</v>
       </c>
       <c r="AC7" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>55</v>
@@ -1585,7 +1561,7 @@
         <v>100011</v>
       </c>
       <c r="E8" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C8,7) + BIN2DEC($D8)))</f>
+        <f t="shared" si="1"/>
         <v>0xA3</v>
       </c>
       <c r="F8" s="3" t="s">
@@ -1601,10 +1577,10 @@
         <v>17</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="K8" s="23" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="L8" s="6">
         <v>0</v>
@@ -1649,7 +1625,7 @@
         <v>73</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="AA8" s="25" t="s">
         <v>41</v>
@@ -1658,12 +1634,12 @@
         <v>69</v>
       </c>
       <c r="AC8" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B9" s="18" t="s">
         <v>55</v>
@@ -1675,7 +1651,7 @@
         <v>100100</v>
       </c>
       <c r="E9" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C9,7) + BIN2DEC($D9)))</f>
+        <f t="shared" si="1"/>
         <v>0xA4</v>
       </c>
       <c r="F9" s="3" t="s">
@@ -1691,7 +1667,7 @@
         <v>17</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="K9" s="23" t="s">
         <v>70</v>
@@ -1739,7 +1715,7 @@
         <v>73</v>
       </c>
       <c r="Z9" s="3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="AA9" s="25" t="s">
         <v>41</v>
@@ -1748,12 +1724,12 @@
         <v>69</v>
       </c>
       <c r="AC9" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>55</v>
@@ -1765,7 +1741,7 @@
         <v>100101</v>
       </c>
       <c r="E10" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C10,7) + BIN2DEC($D10)))</f>
+        <f t="shared" si="1"/>
         <v>0xA5</v>
       </c>
       <c r="F10" s="3" t="s">
@@ -1781,10 +1757,10 @@
         <v>17</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="K10" s="23" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="L10" s="6">
         <v>0</v>
@@ -1829,7 +1805,7 @@
         <v>73</v>
       </c>
       <c r="Z10" s="3" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="AA10" s="25" t="s">
         <v>41</v>
@@ -1838,12 +1814,12 @@
         <v>69</v>
       </c>
       <c r="AC10" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="19" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B11" s="18" t="s">
         <v>55</v>
@@ -1855,7 +1831,7 @@
         <v>100110</v>
       </c>
       <c r="E11" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C11,7) + BIN2DEC($D11)))</f>
+        <f t="shared" si="1"/>
         <v>0xA6</v>
       </c>
       <c r="F11" s="3" t="s">
@@ -1871,7 +1847,7 @@
         <v>17</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="K11" s="23" t="s">
         <v>70</v>
@@ -1919,7 +1895,7 @@
         <v>73</v>
       </c>
       <c r="Z11" s="3" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="AA11" s="25" t="s">
         <v>41</v>
@@ -1928,12 +1904,12 @@
         <v>69</v>
       </c>
       <c r="AC11" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B12" s="18" t="s">
         <v>55</v>
@@ -1945,7 +1921,7 @@
         <v>110000</v>
       </c>
       <c r="E12" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C12,7) + BIN2DEC($D12)))</f>
+        <f t="shared" si="1"/>
         <v>0xB0</v>
       </c>
       <c r="F12" s="3" t="s">
@@ -1964,7 +1940,7 @@
         <v>21</v>
       </c>
       <c r="K12" s="23" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="L12" s="6">
         <v>0</v>
@@ -2009,7 +1985,7 @@
         <v>73</v>
       </c>
       <c r="Z12" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="AA12" s="25" t="s">
         <v>41</v>
@@ -2018,12 +1994,12 @@
         <v>69</v>
       </c>
       <c r="AC12" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B13" s="18" t="s">
         <v>55</v>
@@ -2035,7 +2011,7 @@
         <v>110001</v>
       </c>
       <c r="E13" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C13,7) + BIN2DEC($D13)))</f>
+        <f t="shared" si="1"/>
         <v>0xB1</v>
       </c>
       <c r="F13" s="3" t="s">
@@ -2099,7 +2075,7 @@
         <v>73</v>
       </c>
       <c r="Z13" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="AA13" s="25" t="s">
         <v>41</v>
@@ -2108,12 +2084,12 @@
         <v>69</v>
       </c>
       <c r="AC13" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>55</v>
@@ -2125,7 +2101,7 @@
         <v>110010</v>
       </c>
       <c r="E14" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C14,7) + BIN2DEC($D14)))</f>
+        <f t="shared" si="1"/>
         <v>0xB2</v>
       </c>
       <c r="F14" s="3" t="s">
@@ -2141,7 +2117,7 @@
         <v>17</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>71</v>
@@ -2189,7 +2165,7 @@
         <v>73</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="AA14" s="25" t="s">
         <v>41</v>
@@ -2198,12 +2174,12 @@
         <v>69</v>
       </c>
       <c r="AC14" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>55</v>
@@ -2215,7 +2191,7 @@
         <v>110100</v>
       </c>
       <c r="E15" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C15,7) + BIN2DEC($D15)))</f>
+        <f t="shared" si="1"/>
         <v>0xB4</v>
       </c>
       <c r="F15" s="3" t="s">
@@ -2234,7 +2210,7 @@
         <v>21</v>
       </c>
       <c r="K15" s="23" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="L15" s="6">
         <v>0</v>
@@ -2279,7 +2255,7 @@
         <v>73</v>
       </c>
       <c r="Z15" s="3" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="AA15" s="25" t="s">
         <v>41</v>
@@ -2288,12 +2264,12 @@
         <v>69</v>
       </c>
       <c r="AC15" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B16" s="18" t="s">
         <v>55</v>
@@ -2305,7 +2281,7 @@
         <v>110101</v>
       </c>
       <c r="E16" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C16,7) + BIN2DEC($D16)))</f>
+        <f t="shared" si="1"/>
         <v>0xB5</v>
       </c>
       <c r="F16" s="3" t="s">
@@ -2369,7 +2345,7 @@
         <v>73</v>
       </c>
       <c r="Z16" s="3" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="AA16" s="25" t="s">
         <v>41</v>
@@ -2378,12 +2354,12 @@
         <v>69</v>
       </c>
       <c r="AC16" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>55</v>
@@ -2395,7 +2371,7 @@
         <v>110110</v>
       </c>
       <c r="E17" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C17,7) + BIN2DEC($D17)))</f>
+        <f t="shared" si="1"/>
         <v>0xB6</v>
       </c>
       <c r="F17" s="3" t="s">
@@ -2411,7 +2387,7 @@
         <v>17</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="K17" s="23" t="s">
         <v>71</v>
@@ -2459,7 +2435,7 @@
         <v>73</v>
       </c>
       <c r="Z17" s="3" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="AA17" s="25" t="s">
         <v>41</v>
@@ -2468,12 +2444,12 @@
         <v>69</v>
       </c>
       <c r="AC17" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>85</v>
+        <v>142</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>55</v>
@@ -2482,11 +2458,11 @@
         <v>1</v>
       </c>
       <c r="D18" s="10">
-        <v>1001</v>
+        <v>1110</v>
       </c>
       <c r="E18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>0x89</v>
+        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C18,7) + BIN2DEC($D18)))</f>
+        <v>0x8E</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>17</v>
@@ -2501,16 +2477,16 @@
         <v>17</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="K18" s="23" t="s">
         <v>71</v>
       </c>
       <c r="L18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="6">
         <v>0</v>
@@ -2519,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="6">
         <v>0</v>
@@ -2531,7 +2507,7 @@
         <v>0</v>
       </c>
       <c r="T18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U18" s="6">
         <v>0</v>
@@ -2549,7 +2525,7 @@
         <v>73</v>
       </c>
       <c r="Z18" s="3" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="AA18" s="25" t="s">
         <v>41</v>
@@ -2558,12 +2534,12 @@
         <v>69</v>
       </c>
       <c r="AC18" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
-        <v>82</v>
+      <c r="A19" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>55</v>
@@ -2572,11 +2548,11 @@
         <v>1</v>
       </c>
       <c r="D19" s="10">
-        <v>1010</v>
+        <v>1111</v>
       </c>
       <c r="E19" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C19,7) + BIN2DEC($D19)))</f>
-        <v>0x8A</v>
+        <f t="shared" si="0"/>
+        <v>0x8F</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>17</v>
@@ -2591,10 +2567,10 @@
         <v>17</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="K19" s="23" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="L19" s="6">
         <v>1</v>
@@ -2609,28 +2585,28 @@
         <v>0</v>
       </c>
       <c r="P19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" s="6">
         <v>1</v>
       </c>
       <c r="U19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W19" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X19" s="13" t="s">
         <v>68</v>
@@ -2639,7 +2615,7 @@
         <v>73</v>
       </c>
       <c r="Z19" s="3" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="AA19" s="25" t="s">
         <v>41</v>
@@ -2648,121 +2624,59 @@
         <v>69</v>
       </c>
       <c r="AC19" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="3">
-        <v>1</v>
-      </c>
-      <c r="D20" s="10">
-        <v>1100</v>
-      </c>
-      <c r="E20" s="3" t="str">
-        <f>_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C20,7) + BIN2DEC($D20)))</f>
-        <v>0x8C</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="K20" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="L20" s="6">
-        <v>1</v>
-      </c>
-      <c r="M20" s="6">
-        <v>1</v>
-      </c>
-      <c r="N20" s="6">
-        <v>0</v>
-      </c>
-      <c r="O20" s="6">
-        <v>0</v>
-      </c>
-      <c r="P20" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="6">
-        <v>0</v>
-      </c>
-      <c r="R20" s="6">
-        <v>0</v>
-      </c>
-      <c r="S20" s="6">
-        <v>0</v>
-      </c>
-      <c r="T20" s="6">
-        <v>1</v>
-      </c>
-      <c r="U20" s="6">
-        <v>0</v>
-      </c>
-      <c r="V20" s="6">
-        <v>0</v>
-      </c>
-      <c r="W20" s="16">
-        <v>0</v>
-      </c>
-      <c r="X20" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y20" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z20" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA20" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB20" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC20" t="s">
-        <v>84</v>
-      </c>
+    <row r="20" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="17"/>
+      <c r="X20" s="14"/>
+      <c r="Y20" s="24"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="24"/>
     </row>
     <row r="21" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B21" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C21" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="10">
-        <v>1111</v>
+        <v>1000000</v>
       </c>
       <c r="E21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>0x8F</v>
+        <f t="shared" ref="E21:E36" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C21,7) + BIN2DEC($D21)))</f>
+        <v>0x40</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" t="s">
-        <v>17</v>
+        <v>38</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
       </c>
       <c r="H21" s="3" t="s">
         <v>17</v>
@@ -2771,13 +2685,13 @@
         <v>17</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="K21" s="23" t="s">
         <v>41</v>
       </c>
       <c r="L21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M21" s="6">
         <v>1</v>
@@ -2789,79 +2703,141 @@
         <v>0</v>
       </c>
       <c r="P21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V21" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W21" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X21" s="13" t="s">
         <v>68</v>
       </c>
       <c r="Y21" s="22" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="Z21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AA21" s="25" t="s">
+      <c r="AA21" s="23" t="s">
         <v>41</v>
       </c>
       <c r="AB21" t="s">
         <v>69</v>
       </c>
       <c r="AC21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:29" s="8" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
-      <c r="W22" s="17"/>
-      <c r="X22" s="14"/>
-      <c r="Y22" s="24"/>
-      <c r="Z22" s="7"/>
-      <c r="AA22" s="24"/>
+    <row r="22" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="3">
+        <v>0</v>
+      </c>
+      <c r="D22" s="10">
+        <v>1000010</v>
+      </c>
+      <c r="E22" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0x42</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="L22" s="6">
+        <v>0</v>
+      </c>
+      <c r="M22" s="6">
+        <v>1</v>
+      </c>
+      <c r="N22" s="6">
+        <v>0</v>
+      </c>
+      <c r="O22" s="6">
+        <v>0</v>
+      </c>
+      <c r="P22" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>0</v>
+      </c>
+      <c r="R22" s="6">
+        <v>0</v>
+      </c>
+      <c r="S22" s="6">
+        <v>0</v>
+      </c>
+      <c r="T22" s="6">
+        <v>0</v>
+      </c>
+      <c r="U22" s="6">
+        <v>0</v>
+      </c>
+      <c r="V22" s="6">
+        <v>0</v>
+      </c>
+      <c r="W22" s="16">
+        <v>0</v>
+      </c>
+      <c r="X22" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y22" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA22" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="23" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>55</v>
@@ -2870,17 +2846,17 @@
         <v>0</v>
       </c>
       <c r="D23" s="10">
-        <v>1000000</v>
+        <v>1000100</v>
       </c>
       <c r="E23" s="3" t="str">
-        <f t="shared" ref="E23:E38" si="1">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C23,7) + BIN2DEC($D23)))</f>
-        <v>0x40</v>
+        <f t="shared" si="2"/>
+        <v>0x44</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="G23" t="s">
+        <v>17</v>
       </c>
       <c r="H23" s="3" t="s">
         <v>17</v>
@@ -2895,10 +2871,10 @@
         <v>41</v>
       </c>
       <c r="L23" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N23" s="6">
         <v>0</v>
@@ -2946,12 +2922,12 @@
         <v>69</v>
       </c>
       <c r="AC23" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>55</v>
@@ -2960,17 +2936,17 @@
         <v>0</v>
       </c>
       <c r="D24" s="10">
-        <v>1000010</v>
+        <v>1000101</v>
       </c>
       <c r="E24" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x42</v>
+        <f t="shared" si="2"/>
+        <v>0x45</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24">
-        <v>2</v>
+        <v>17</v>
+      </c>
+      <c r="G24" t="s">
+        <v>17</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>17</v>
@@ -2985,10 +2961,10 @@
         <v>41</v>
       </c>
       <c r="L24" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N24" s="6">
         <v>0</v>
@@ -3036,12 +3012,12 @@
         <v>69</v>
       </c>
       <c r="AC24" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>28</v>
+      <c r="A25" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>55</v>
@@ -3050,11 +3026,11 @@
         <v>0</v>
       </c>
       <c r="D25" s="10">
-        <v>1000100</v>
+        <v>10000</v>
       </c>
       <c r="E25" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x44</v>
+        <f t="shared" si="2"/>
+        <v>0x10</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>17</v>
@@ -3075,7 +3051,7 @@
         <v>41</v>
       </c>
       <c r="L25" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M25" s="6">
         <v>0</v>
@@ -3087,7 +3063,7 @@
         <v>0</v>
       </c>
       <c r="P25" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="6">
         <v>0</v>
@@ -3117,21 +3093,21 @@
         <v>74</v>
       </c>
       <c r="Z25" s="3" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="AA25" s="23" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="AB25" t="s">
         <v>69</v>
       </c>
       <c r="AC25" t="s">
-        <v>44</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>29</v>
+      <c r="A26" s="19" t="s">
+        <v>82</v>
       </c>
       <c r="B26" s="18" t="s">
         <v>55</v>
@@ -3140,11 +3116,11 @@
         <v>0</v>
       </c>
       <c r="D26" s="10">
-        <v>1000101</v>
+        <v>10001</v>
       </c>
       <c r="E26" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x45</v>
+        <f t="shared" si="2"/>
+        <v>0x11</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>17</v>
@@ -3165,7 +3141,7 @@
         <v>41</v>
       </c>
       <c r="L26" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" s="6">
         <v>0</v>
@@ -3177,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="P26" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="6">
         <v>0</v>
@@ -3207,21 +3183,21 @@
         <v>74</v>
       </c>
       <c r="Z26" s="3" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="AA26" s="23" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="AB26" t="s">
         <v>69</v>
       </c>
       <c r="AC26" t="s">
-        <v>44</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="19" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B27" s="18" t="s">
         <v>55</v>
@@ -3230,11 +3206,11 @@
         <v>0</v>
       </c>
       <c r="D27" s="10">
-        <v>10000</v>
+        <v>10010</v>
       </c>
       <c r="E27" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x10</v>
+        <f t="shared" si="2"/>
+        <v>0x12</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>17</v>
@@ -3297,21 +3273,21 @@
         <v>74</v>
       </c>
       <c r="Z27" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="AA27" s="23" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AB27" t="s">
         <v>69</v>
       </c>
       <c r="AC27" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="19" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>55</v>
@@ -3320,11 +3296,11 @@
         <v>0</v>
       </c>
       <c r="D28" s="10">
-        <v>10001</v>
+        <v>10011</v>
       </c>
       <c r="E28" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x11</v>
+        <f t="shared" si="2"/>
+        <v>0x13</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>17</v>
@@ -3387,21 +3363,21 @@
         <v>74</v>
       </c>
       <c r="Z28" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="AA28" s="23" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="AB28" t="s">
         <v>69</v>
       </c>
       <c r="AC28" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>55</v>
@@ -3410,11 +3386,11 @@
         <v>0</v>
       </c>
       <c r="D29" s="10">
-        <v>10010</v>
+        <v>10100</v>
       </c>
       <c r="E29" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x12</v>
+        <f t="shared" si="2"/>
+        <v>0x14</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>17</v>
@@ -3477,21 +3453,21 @@
         <v>74</v>
       </c>
       <c r="Z29" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="AA29" s="23" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="AB29" t="s">
         <v>69</v>
       </c>
       <c r="AC29" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B30" s="18" t="s">
         <v>55</v>
@@ -3500,11 +3476,11 @@
         <v>0</v>
       </c>
       <c r="D30" s="10">
-        <v>10011</v>
+        <v>10101</v>
       </c>
       <c r="E30" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x13</v>
+        <f t="shared" si="2"/>
+        <v>0x15</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>17</v>
@@ -3567,21 +3543,21 @@
         <v>74</v>
       </c>
       <c r="Z30" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="AA30" s="23" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="AB30" t="s">
         <v>69</v>
       </c>
       <c r="AC30" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B31" s="18" t="s">
         <v>55</v>
@@ -3590,11 +3566,11 @@
         <v>0</v>
       </c>
       <c r="D31" s="10">
-        <v>10100</v>
+        <v>10110</v>
       </c>
       <c r="E31" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x14</v>
+        <f t="shared" si="2"/>
+        <v>0x16</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>17</v>
@@ -3657,21 +3633,21 @@
         <v>74</v>
       </c>
       <c r="Z31" s="3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="AA31" s="23" t="s">
-        <v>140</v>
+        <v>78</v>
       </c>
       <c r="AB31" t="s">
         <v>69</v>
       </c>
       <c r="AC31" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="B32" s="18" t="s">
         <v>55</v>
@@ -3680,11 +3656,10 @@
         <v>0</v>
       </c>
       <c r="D32" s="10">
-        <v>10101</v>
-      </c>
-      <c r="E32" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x15</v>
+        <v>100001</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>17</v>
@@ -3695,13 +3670,13 @@
       <c r="H32" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I32" s="13" t="s">
+      <c r="I32" t="s">
         <v>17</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="23" t="s">
+      <c r="K32" s="3" t="s">
         <v>41</v>
       </c>
       <c r="L32" s="6">
@@ -3737,31 +3712,31 @@
       <c r="V32" s="6">
         <v>0</v>
       </c>
-      <c r="W32" s="16">
-        <v>0</v>
-      </c>
-      <c r="X32" s="13" t="s">
+      <c r="W32" s="6">
+        <v>0</v>
+      </c>
+      <c r="X32" t="s">
         <v>68</v>
       </c>
-      <c r="Y32" s="22" t="s">
+      <c r="Y32" s="3" t="s">
         <v>74</v>
       </c>
       <c r="Z32" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA32" s="23" t="s">
-        <v>141</v>
+        <v>92</v>
+      </c>
+      <c r="AA32" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="AB32" t="s">
         <v>69</v>
       </c>
       <c r="AC32" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="19" t="s">
-        <v>97</v>
+      <c r="A33" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="B33" s="18" t="s">
         <v>55</v>
@@ -3770,11 +3745,11 @@
         <v>0</v>
       </c>
       <c r="D33" s="10">
-        <v>10110</v>
+        <v>1110000</v>
       </c>
       <c r="E33" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x16</v>
+        <f t="shared" si="2"/>
+        <v>0x70</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>17</v>
@@ -3795,10 +3770,10 @@
         <v>41</v>
       </c>
       <c r="L33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N33" s="6">
         <v>0</v>
@@ -3810,25 +3785,25 @@
         <v>1</v>
       </c>
       <c r="Q33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V33" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W33" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X33" s="13" t="s">
         <v>68</v>
@@ -3837,21 +3812,21 @@
         <v>74</v>
       </c>
       <c r="Z33" s="3" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="AA33" s="23" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="AB33" t="s">
         <v>69</v>
       </c>
       <c r="AC33" t="s">
-        <v>150</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
-        <v>143</v>
+      <c r="A34" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>55</v>
@@ -3860,10 +3835,11 @@
         <v>0</v>
       </c>
       <c r="D34" s="10">
-        <v>100001</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>142</v>
+        <v>1110001</v>
+      </c>
+      <c r="E34" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>0x71</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>17</v>
@@ -3874,20 +3850,20 @@
       <c r="H34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="13" t="s">
         <v>17</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K34" s="3" t="s">
+      <c r="K34" s="23" t="s">
         <v>41</v>
       </c>
       <c r="L34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34" s="6">
         <v>0</v>
@@ -3899,48 +3875,48 @@
         <v>1</v>
       </c>
       <c r="Q34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U34" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V34" s="6">
-        <v>0</v>
-      </c>
-      <c r="W34" s="6">
-        <v>0</v>
-      </c>
-      <c r="X34" t="s">
+        <v>1</v>
+      </c>
+      <c r="W34" s="16">
+        <v>1</v>
+      </c>
+      <c r="X34" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="Y34" s="3" t="s">
+      <c r="Y34" s="22" t="s">
         <v>74</v>
       </c>
       <c r="Z34" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA34" s="3" t="s">
-        <v>79</v>
+        <v>41</v>
+      </c>
+      <c r="AA34" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="AB34" t="s">
         <v>69</v>
       </c>
       <c r="AC34" t="s">
-        <v>151</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B35" s="18" t="s">
         <v>55</v>
@@ -3949,11 +3925,11 @@
         <v>0</v>
       </c>
       <c r="D35" s="10">
-        <v>1110000</v>
+        <v>1110010</v>
       </c>
       <c r="E35" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x70</v>
+        <f t="shared" si="2"/>
+        <v>0x72</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>17</v>
@@ -4025,12 +4001,12 @@
         <v>69</v>
       </c>
       <c r="AC35" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>55</v>
@@ -4039,11 +4015,11 @@
         <v>0</v>
       </c>
       <c r="D36" s="10">
-        <v>1110001</v>
+        <v>1110011</v>
       </c>
       <c r="E36" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x71</v>
+        <f t="shared" si="2"/>
+        <v>0x73</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>17</v>
@@ -4115,12 +4091,12 @@
         <v>69</v>
       </c>
       <c r="AC36" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>55</v>
@@ -4129,11 +4105,11 @@
         <v>0</v>
       </c>
       <c r="D37" s="10">
-        <v>1110010</v>
+        <v>1110100</v>
       </c>
       <c r="E37" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x72</v>
+        <f t="shared" ref="E37:E38" si="3">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C37,7) + BIN2DEC($D37)))</f>
+        <v>0x74</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>17</v>
@@ -4205,12 +4181,12 @@
         <v>69</v>
       </c>
       <c r="AC37" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>55</v>
@@ -4219,11 +4195,11 @@
         <v>0</v>
       </c>
       <c r="D38" s="10">
-        <v>1110011</v>
+        <v>1111000</v>
       </c>
       <c r="E38" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x73</v>
+        <f t="shared" si="3"/>
+        <v>0x78</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>17</v>
@@ -4295,186 +4271,6 @@
         <v>69</v>
       </c>
       <c r="AC38" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" s="3">
-        <v>0</v>
-      </c>
-      <c r="D39" s="10">
-        <v>1110100</v>
-      </c>
-      <c r="E39" s="3" t="str">
-        <f t="shared" ref="E39:E40" si="2">_xlfn.CONCAT("0x", DEC2HEX(_xlfn.BITLSHIFT($C39,7) + BIN2DEC($D39)))</f>
-        <v>0x74</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" t="s">
-        <v>17</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="L39" s="6">
-        <v>1</v>
-      </c>
-      <c r="M39" s="6">
-        <v>1</v>
-      </c>
-      <c r="N39" s="6">
-        <v>0</v>
-      </c>
-      <c r="O39" s="6">
-        <v>0</v>
-      </c>
-      <c r="P39" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q39" s="6">
-        <v>1</v>
-      </c>
-      <c r="R39" s="6">
-        <v>1</v>
-      </c>
-      <c r="S39" s="6">
-        <v>1</v>
-      </c>
-      <c r="T39" s="6">
-        <v>1</v>
-      </c>
-      <c r="U39" s="6">
-        <v>1</v>
-      </c>
-      <c r="V39" s="6">
-        <v>1</v>
-      </c>
-      <c r="W39" s="16">
-        <v>1</v>
-      </c>
-      <c r="X39" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y39" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z39" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA39" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB39" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:29" ht="16" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C40" s="3">
-        <v>0</v>
-      </c>
-      <c r="D40" s="10">
-        <v>1111000</v>
-      </c>
-      <c r="E40" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>0x78</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" t="s">
-        <v>17</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I40" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="J40" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K40" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="L40" s="6">
-        <v>1</v>
-      </c>
-      <c r="M40" s="6">
-        <v>1</v>
-      </c>
-      <c r="N40" s="6">
-        <v>0</v>
-      </c>
-      <c r="O40" s="6">
-        <v>0</v>
-      </c>
-      <c r="P40" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q40" s="6">
-        <v>1</v>
-      </c>
-      <c r="R40" s="6">
-        <v>1</v>
-      </c>
-      <c r="S40" s="6">
-        <v>1</v>
-      </c>
-      <c r="T40" s="6">
-        <v>1</v>
-      </c>
-      <c r="U40" s="6">
-        <v>1</v>
-      </c>
-      <c r="V40" s="6">
-        <v>1</v>
-      </c>
-      <c r="W40" s="16">
-        <v>1</v>
-      </c>
-      <c r="X40" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="Y40" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="Z40" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA40" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB40" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC40" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>